<commit_message>
* IHM quasiement fini, reste les interactions à ecrire
</commit_message>
<xml_diff>
--- a/code/Console-Pilotage/TouchGFX/assets/texts/texts.xlsx
+++ b/code/Console-Pilotage/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2094" uniqueCount="106">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -183,6 +183,200 @@
   </si>
   <si>
     <t xml:space="preserve">0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sélection
+du voilier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sélection
+du voilier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sélection
+du voilier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sélection
+du voilier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sélection
+du voilier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sélection
+du voilier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sélection
+du voilier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sélection
+du voilier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sélection
+du voilier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ca marche</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sélection
+du voilier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sélection
+du voilier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sélection
+du voilier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sélection
+du voilier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sélection
+du voilier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sélection
+du voilier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sélection
+du voilier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sélection
+du voilier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sélection
+du voilier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sélection
+du voilier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sélection
+du voilier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sélection
+du voilier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sélection
+du voilier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sélection
+du voilier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sélection
+du voilier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sélection
+du voilier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sélection
+du voilier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sélection
+du voilier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sélection
+du voilier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sélection
+du voilier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sélection
+du voilier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sélection
+du voilier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sélection
+du voilier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sélection
+du voilier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sélection
+du voilier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sélection
+du voilier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sélection
+du voilier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sélection
+du voilier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sélection
+du voilier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sélection
+du voilier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sélection
+du voilier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sélection
+du voilier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sélection
+du voilier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sélection
+du voilier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sélection
+du voilier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt;%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
   </si>
 </sst>
 </file>
@@ -1424,9 +1618,13 @@
       <c r="F4" t="s">
         <v>17</v>
       </c>
-      <c r="G4"/>
+      <c r="G4" t="s">
+        <v>105</v>
+      </c>
       <c r="H4"/>
-      <c r="I4"/>
+      <c r="I4" t="s">
+        <v>43</v>
+      </c>
       <c r="J4"/>
       <c r="L4" s="4" t="s">
         <v>9</v>
@@ -1666,7 +1864,7 @@
     </row>
     <row r="4">
       <c r="B4" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
         <v>38</v>
@@ -1678,58 +1876,92 @@
         <v>46</v>
       </c>
       <c r="F4" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D5" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E5" t="s">
         <v>46</v>
       </c>
       <c r="F5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C6" t="s">
         <v>42</v>
       </c>
       <c r="D6" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E6" t="s">
         <v>46</v>
       </c>
       <c r="F6" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D7" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E7" t="s">
         <v>46</v>
       </c>
       <c r="F7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="s">
+        <v>103</v>
+      </c>
+      <c r="C8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" t="s">
         <v>55</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="s">
+        <v>104</v>
+      </c>
+      <c r="C9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
* Dernier prototype de l'IHM, a valider par la team
</commit_message>
<xml_diff>
--- a/code/Console-Pilotage/TouchGFX/assets/texts/texts.xlsx
+++ b/code/Console-Pilotage/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2094" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2499" uniqueCount="113">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -377,6 +377,27 @@
   </si>
   <si>
     <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a-Z,0-9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">?!,;:./&amp;é"'(-è_çà)#{[|`\^@]}=+~*$ù%µ&lt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a-z,A-Z,0-9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a-z</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &amp;é"'(-è_çà)=~#{[|`\^@]}°+&gt;,;:!?./§ù*^$%µ£¨</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">_</t>
   </si>
 </sst>
 </file>
@@ -1690,11 +1711,15 @@
         <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6"/>
+        <v>112</v>
+      </c>
+      <c r="G6" t="s">
+        <v>110</v>
+      </c>
       <c r="H6"/>
-      <c r="I6"/>
+      <c r="I6" t="s">
+        <v>108</v>
+      </c>
       <c r="J6"/>
       <c r="L6" s="7" t="s">
         <v>2</v>

</xml_diff>